<commit_message>
ADD: Lab 2 Sweep Data and code
</commit_message>
<xml_diff>
--- a/Lab2/CalibrationData.xlsx
+++ b/Lab2/CalibrationData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Distance (cm)</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Prediction</t>
+  </si>
+  <si>
+    <t>Calculated Distance</t>
+  </si>
+  <si>
+    <t>Did not include</t>
   </si>
 </sst>
 </file>
@@ -216,11 +222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84635008"/>
-        <c:axId val="84634432"/>
+        <c:axId val="87245952"/>
+        <c:axId val="87246528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84635008"/>
+        <c:axId val="87245952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -230,12 +236,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84634432"/>
+        <c:crossAx val="87246528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84634432"/>
+        <c:axId val="87246528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -246,7 +252,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84635008"/>
+        <c:crossAx val="87245952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -412,11 +418,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72593344"/>
-        <c:axId val="53091648"/>
+        <c:axId val="87248256"/>
+        <c:axId val="87248832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72593344"/>
+        <c:axId val="87248256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,12 +432,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53091648"/>
+        <c:crossAx val="87248832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53091648"/>
+        <c:axId val="87248832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72593344"/>
+        <c:crossAx val="87248256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -468,16 +474,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -819,7 +825,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,6 +846,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -852,6 +861,9 @@
         <f>B2/255*5</f>
         <v>1.9607843137254901</v>
       </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -864,6 +876,9 @@
         <f t="shared" ref="C3:C11" si="0">B3/255*5</f>
         <v>2.1960784313725492</v>
       </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -876,6 +891,10 @@
         <f t="shared" si="0"/>
         <v>2.8431372549019605</v>
       </c>
+      <c r="D4">
+        <f>(LN(C4) - LN(4.2223))/-0.024</f>
+        <v>16.477995565703498</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -888,6 +907,10 @@
         <f t="shared" si="0"/>
         <v>2.6470588235294117</v>
       </c>
+      <c r="D5">
+        <f>(LN(C5) - LN(4.2223))/-0.024</f>
+        <v>19.455452398292863</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -900,6 +923,10 @@
         <f t="shared" si="0"/>
         <v>2.4313725490196076</v>
       </c>
+      <c r="D6">
+        <f>(LN(C6) - LN(4.2223))/-0.024</f>
+        <v>22.996836266350893</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -912,6 +939,10 @@
         <f t="shared" si="0"/>
         <v>2.0980392156862746</v>
       </c>
+      <c r="D7">
+        <f>(LN(C7) - LN(4.2223))/-0.024</f>
+        <v>29.140700063981331</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -924,6 +955,10 @@
         <f t="shared" si="0"/>
         <v>1.8431372549019609</v>
       </c>
+      <c r="D8">
+        <f>(LN(C8) - LN(4.2223))/-0.024</f>
+        <v>34.537952238643925</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -936,6 +971,10 @@
         <f t="shared" si="0"/>
         <v>1.588235294117647</v>
       </c>
+      <c r="D9">
+        <f>(LN(C9) - LN(4.2223))/-0.024</f>
+        <v>40.739853388542478</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -948,6 +987,10 @@
         <f t="shared" si="0"/>
         <v>1.4313725490196076</v>
       </c>
+      <c r="D10">
+        <f>(LN(C10) - LN(4.2223))/-0.024</f>
+        <v>45.072758118711135</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -960,6 +1003,10 @@
         <f t="shared" si="0"/>
         <v>1.2941176470588236</v>
       </c>
+      <c r="D11">
+        <f>(LN(C11) - LN(4.2223))/-0.024</f>
+        <v>49.272953915459688</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1003,7 +1050,7 @@
         <v>2.5098039215686274</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D23" si="2">4.2223*(EXP(1)^(-1*0.024*A15))</f>
+        <f t="shared" ref="D15:D18" si="2">4.2223*(EXP(1)^(-1*0.024*A15))</f>
         <v>2.4902422708487379</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UPDATE: finished up single sweep and two axis sweep with visualization
adding calibration info

still need to clean up code and add comments
</commit_message>
<xml_diff>
--- a/Lab2/CalibrationData.xlsx
+++ b/Lab2/CalibrationData.xlsx
@@ -30,19 +30,19 @@
     <t>NEW DISTANCES</t>
   </si>
   <si>
-    <t>Output</t>
+    <t>Did not include</t>
   </si>
   <si>
-    <t>Voltage</t>
+    <t>Output (max 255)</t>
   </si>
   <si>
-    <t>Prediction</t>
+    <t>Calculated Distance (cm)</t>
   </si>
   <si>
-    <t>Calculated Distance</t>
+    <t>Predicted Distance (cm)</t>
   </si>
   <si>
-    <t>Did not include</t>
+    <t>Voltage (max 5V)</t>
   </si>
 </sst>
 </file>
@@ -108,6 +108,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -127,6 +131,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Calibration Readings (V)</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -222,37 +229,85 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87245952"/>
-        <c:axId val="87246528"/>
+        <c:axId val="65304192"/>
+        <c:axId val="65304768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87245952"/>
+        <c:axId val="65304192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance Set</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> From Infrared Sensor (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87246528"/>
+        <c:crossAx val="65304768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87246528"/>
+        <c:axId val="65304768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sensor</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>  Output (V)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87245952"/>
+        <c:crossAx val="65304192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -288,6 +343,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Calibration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Error Plot</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -297,6 +376,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual Output</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -355,6 +437,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Predicted Output</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -418,37 +503,75 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="87248256"/>
-        <c:axId val="87248832"/>
+        <c:axId val="53460992"/>
+        <c:axId val="53461568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87248256"/>
+        <c:axId val="53460992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance Set From Infrared Sensor (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87248832"/>
+        <c:crossAx val="53461568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87248832"/>
+        <c:axId val="53461568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sensor Output (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87248256"/>
+        <c:crossAx val="53460992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -475,15 +598,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:colOff>555625</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>36511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -504,16 +627,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>106362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>269875</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -824,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F19" sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +970,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -862,7 +985,7 @@
         <v>1.9607843137254901</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -877,7 +1000,7 @@
         <v>2.1960784313725492</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,7 +1015,7 @@
         <v>2.8431372549019605</v>
       </c>
       <c r="D4">
-        <f>(LN(C4) - LN(4.2223))/-0.024</f>
+        <f t="shared" ref="D4:D11" si="1">(LN(C4) - LN(4.2223))/-0.024</f>
         <v>16.477995565703498</v>
       </c>
     </row>
@@ -908,7 +1031,7 @@
         <v>2.6470588235294117</v>
       </c>
       <c r="D5">
-        <f>(LN(C5) - LN(4.2223))/-0.024</f>
+        <f t="shared" si="1"/>
         <v>19.455452398292863</v>
       </c>
     </row>
@@ -924,7 +1047,7 @@
         <v>2.4313725490196076</v>
       </c>
       <c r="D6">
-        <f>(LN(C6) - LN(4.2223))/-0.024</f>
+        <f t="shared" si="1"/>
         <v>22.996836266350893</v>
       </c>
     </row>
@@ -940,7 +1063,7 @@
         <v>2.0980392156862746</v>
       </c>
       <c r="D7">
-        <f>(LN(C7) - LN(4.2223))/-0.024</f>
+        <f t="shared" si="1"/>
         <v>29.140700063981331</v>
       </c>
     </row>
@@ -956,7 +1079,7 @@
         <v>1.8431372549019609</v>
       </c>
       <c r="D8">
-        <f>(LN(C8) - LN(4.2223))/-0.024</f>
+        <f t="shared" si="1"/>
         <v>34.537952238643925</v>
       </c>
     </row>
@@ -972,7 +1095,7 @@
         <v>1.588235294117647</v>
       </c>
       <c r="D9">
-        <f>(LN(C9) - LN(4.2223))/-0.024</f>
+        <f t="shared" si="1"/>
         <v>40.739853388542478</v>
       </c>
     </row>
@@ -988,7 +1111,7 @@
         <v>1.4313725490196076</v>
       </c>
       <c r="D10">
-        <f>(LN(C10) - LN(4.2223))/-0.024</f>
+        <f t="shared" si="1"/>
         <v>45.072758118711135</v>
       </c>
     </row>
@@ -1004,7 +1127,7 @@
         <v>1.2941176470588236</v>
       </c>
       <c r="D11">
-        <f>(LN(C11) - LN(4.2223))/-0.024</f>
+        <f t="shared" si="1"/>
         <v>49.272953915459688</v>
       </c>
     </row>
@@ -1013,13 +1136,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,11 +1169,11 @@
         <v>128</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:C18" si="1">B15/255*5</f>
+        <f t="shared" ref="C15:C18" si="2">B15/255*5</f>
         <v>2.5098039215686274</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D18" si="2">4.2223*(EXP(1)^(-1*0.024*A15))</f>
+        <f t="shared" ref="D15:D18" si="3">4.2223*(EXP(1)^(-1*0.024*A15))</f>
         <v>2.4902422708487379</v>
       </c>
     </row>
@@ -1062,11 +1185,11 @@
         <v>114</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2352941176470589</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.2086467623926889</v>
       </c>
     </row>
@@ -1078,11 +1201,11 @@
         <v>61</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.196078431372549</v>
       </c>
       <c r="D17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1279253854904099</v>
       </c>
     </row>
@@ -1094,11 +1217,11 @@
         <v>55</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0784313725490198</v>
       </c>
       <c r="D18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0003800754835228</v>
       </c>
     </row>

</xml_diff>